<commit_message>
app version updated to (version 1.0)
</commit_message>
<xml_diff>
--- a/Students Data.xlsx
+++ b/Students Data.xlsx
@@ -702,22 +702,22 @@
     <t>AGE</t>
   </si>
   <si>
-    <t xml:space="preserve">SCORE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENDER </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TERM </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACADEMIC YEAR </t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>TERM</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>ACADEMIC YEAR</t>
   </si>
 </sst>
 </file>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:F439"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,16 +1057,16 @@
         <v>226</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>17.8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E2" s="1">
         <v>7</v>
@@ -1100,7 +1100,7 @@
         <v>15.2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -1120,7 +1120,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E4" s="1">
         <v>4</v>
@@ -1140,7 +1140,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
@@ -1160,7 +1160,7 @@
         <v>14.5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -1180,7 +1180,7 @@
         <v>10.1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E7" s="1">
         <v>3</v>
@@ -1200,7 +1200,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1220,7 +1220,7 @@
         <v>12.4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
@@ -1240,7 +1240,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -1260,7 +1260,7 @@
         <v>13.2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E11" s="1">
         <v>6</v>
@@ -1280,7 +1280,7 @@
         <v>19.5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
@@ -1300,7 +1300,7 @@
         <v>11.8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -1320,7 +1320,7 @@
         <v>10.6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1340,7 +1340,7 @@
         <v>16.3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E15" s="1">
         <v>8</v>
@@ -1360,7 +1360,7 @@
         <v>14.2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
@@ -1380,7 +1380,7 @@
         <v>5.7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E17" s="1">
         <v>3</v>
@@ -1400,7 +1400,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -1420,7 +1420,7 @@
         <v>13.9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E19" s="1">
         <v>5</v>
@@ -1440,7 +1440,7 @@
         <v>12.3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
@@ -1460,7 +1460,7 @@
         <v>15.4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -1480,7 +1480,7 @@
         <v>17.2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E22" s="1">
         <v>4</v>
@@ -1500,7 +1500,7 @@
         <v>13.4</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
@@ -1520,7 +1520,7 @@
         <v>15.8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E24" s="1">
         <v>6</v>
@@ -1540,7 +1540,7 @@
         <v>11.2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -1560,7 +1560,7 @@
         <v>19.3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E26" s="1">
         <v>4</v>
@@ -1580,7 +1580,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E27" s="1">
         <v>2</v>
@@ -1600,7 +1600,7 @@
         <v>18.899999999999999</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E28" s="1">
         <v>3</v>
@@ -1620,7 +1620,7 @@
         <v>13.1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E29" s="1">
         <v>8</v>
@@ -1640,7 +1640,7 @@
         <v>9.9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E30" s="1">
         <v>3</v>
@@ -1660,7 +1660,7 @@
         <v>14.7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E31" s="1">
         <v>2</v>
@@ -1680,7 +1680,7 @@
         <v>9.4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E32" s="1">
         <v>8</v>
@@ -1700,7 +1700,7 @@
         <v>15.3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E33" s="1">
         <v>2</v>
@@ -1720,7 +1720,7 @@
         <v>18.8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -1740,7 +1740,7 @@
         <v>14.1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E35" s="1">
         <v>7</v>
@@ -1760,7 +1760,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E36" s="1">
         <v>7</v>
@@ -1780,7 +1780,7 @@
         <v>11.5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E37" s="1">
         <v>6</v>
@@ -1800,7 +1800,7 @@
         <v>13.6</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E38" s="1">
         <v>7</v>
@@ -1820,7 +1820,7 @@
         <v>11.4</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E39" s="1">
         <v>3</v>
@@ -1840,7 +1840,7 @@
         <v>17.5</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E40" s="1">
         <v>2</v>
@@ -1860,7 +1860,7 @@
         <v>10.8</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E41" s="1">
         <v>4</v>
@@ -1880,7 +1880,7 @@
         <v>12.1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E42" s="1">
         <v>2</v>
@@ -1900,7 +1900,7 @@
         <v>11.1</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E43" s="1">
         <v>8</v>
@@ -1920,7 +1920,7 @@
         <v>8.9</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E44" s="1">
         <v>3</v>
@@ -1940,7 +1940,7 @@
         <v>10.3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E45" s="1">
         <v>6</v>
@@ -1960,7 +1960,7 @@
         <v>13.7</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E46" s="1">
         <v>8</v>
@@ -1980,7 +1980,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
@@ -2000,7 +2000,7 @@
         <v>12.7</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
@@ -2020,7 +2020,7 @@
         <v>19.8</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E49" s="1">
         <v>2</v>
@@ -2040,7 +2040,7 @@
         <v>8.4</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E50" s="1">
         <v>6</v>
@@ -2060,7 +2060,7 @@
         <v>15.7</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -2080,7 +2080,7 @@
         <v>12.8</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E52" s="1">
         <v>5</v>
@@ -2100,7 +2100,7 @@
         <v>13.5</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E53" s="1">
         <v>3</v>
@@ -2120,7 +2120,7 @@
         <v>10.4</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E54" s="1">
         <v>7</v>
@@ -2140,7 +2140,7 @@
         <v>13.3</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E55" s="1">
         <v>2</v>
@@ -2160,7 +2160,7 @@
         <v>11.3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E56" s="1">
         <v>1</v>
@@ -2180,7 +2180,7 @@
         <v>18.3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E57" s="1">
         <v>6</v>
@@ -2200,7 +2200,7 @@
         <v>13</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E58" s="1">
         <v>8</v>
@@ -2220,7 +2220,7 @@
         <v>14.8</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E59" s="1">
         <v>1</v>
@@ -2240,7 +2240,7 @@
         <v>16.7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E60" s="1">
         <v>7</v>
@@ -2260,7 +2260,7 @@
         <v>11.7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E61" s="1">
         <v>2</v>
@@ -2280,7 +2280,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E62" s="1">
         <v>4</v>
@@ -2300,7 +2300,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E63" s="1">
         <v>3</v>
@@ -2320,7 +2320,7 @@
         <v>14.9</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E64" s="1">
         <v>8</v>
@@ -2340,7 +2340,7 @@
         <v>13.8</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E65" s="1">
         <v>3</v>
@@ -2360,7 +2360,7 @@
         <v>10.9</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -2380,7 +2380,7 @@
         <v>12.2</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E67" s="1">
         <v>2</v>
@@ -2400,7 +2400,7 @@
         <v>19.600000000000001</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E68" s="1">
         <v>8</v>
@@ -2420,7 +2420,7 @@
         <v>11.9</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E69" s="1">
         <v>7</v>
@@ -2440,7 +2440,7 @@
         <v>15.5</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E70" s="1">
         <v>2</v>
@@ -2460,7 +2460,7 @@
         <v>9.5</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
@@ -2480,7 +2480,7 @@
         <v>19.100000000000001</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E72" s="1">
         <v>5</v>
@@ -2500,7 +2500,7 @@
         <v>16.2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E73" s="1">
         <v>3</v>
@@ -2520,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E74" s="1">
         <v>4</v>
@@ -2540,7 +2540,7 @@
         <v>18.7</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E75" s="1">
         <v>7</v>
@@ -2560,7 +2560,7 @@
         <v>8.6</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E76" s="1">
         <v>4</v>
@@ -2580,7 +2580,7 @@
         <v>14.6</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E77" s="1">
         <v>1</v>
@@ -2600,7 +2600,7 @@
         <v>12.6</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E78" s="1">
         <v>8</v>
@@ -2620,7 +2620,7 @@
         <v>9.1</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E79" s="1">
         <v>3</v>
@@ -2640,7 +2640,7 @@
         <v>13.5</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E80" s="1">
         <v>2</v>
@@ -2660,7 +2660,7 @@
         <v>18.2</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E81" s="1">
         <v>7</v>
@@ -2680,7 +2680,7 @@
         <v>15.1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E82" s="1">
         <v>4</v>
@@ -2700,7 +2700,7 @@
         <v>11.6</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E83" s="1">
         <v>8</v>
@@ -2720,7 +2720,7 @@
         <v>7.8</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E84" s="1">
         <v>3</v>
@@ -2740,7 +2740,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E85" s="1">
         <v>8</v>
@@ -2760,7 +2760,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E86" s="1">
         <v>2</v>
@@ -2780,7 +2780,7 @@
         <v>17</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E87" s="1">
         <v>2</v>
@@ -2800,7 +2800,7 @@
         <v>10.5</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E88" s="1">
         <v>4</v>
@@ -2820,7 +2820,7 @@
         <v>18</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E89" s="1">
         <v>8</v>
@@ -2840,7 +2840,7 @@
         <v>9.6</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E90" s="1">
         <v>1</v>
@@ -2860,7 +2860,7 @@
         <v>15.9</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E91" s="1">
         <v>7</v>
@@ -2880,7 +2880,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E92" s="1">
         <v>2</v>
@@ -2900,7 +2900,7 @@
         <v>13</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E93" s="1">
         <v>6</v>
@@ -2920,7 +2920,7 @@
         <v>7.6</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E94" s="1">
         <v>1</v>
@@ -2940,7 +2940,7 @@
         <v>14</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E95" s="1">
         <v>3</v>
@@ -2960,7 +2960,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E96" s="1">
         <v>7</v>
@@ -2980,7 +2980,7 @@
         <v>16.8</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E97" s="1">
         <v>6</v>
@@ -3000,7 +3000,7 @@
         <v>11.9</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E98" s="1">
         <v>3</v>
@@ -3020,7 +3020,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E99" s="1">
         <v>4</v>
@@ -3040,7 +3040,7 @@
         <v>17.3</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E100" s="1">
         <v>2</v>
@@ -3060,7 +3060,7 @@
         <v>12</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E101" s="1">
         <v>8</v>
@@ -3080,7 +3080,7 @@
         <v>10.7</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E102" s="1">
         <v>7</v>
@@ -3100,7 +3100,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E103" s="1">
         <v>3</v>
@@ -3120,7 +3120,7 @@
         <v>7.9</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E104" s="1">
         <v>6</v>
@@ -3140,7 +3140,7 @@
         <v>11</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E105" s="1">
         <v>8</v>
@@ -3160,7 +3160,7 @@
         <v>14.3</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E106" s="1">
         <v>1</v>
@@ -3180,7 +3180,7 @@
         <v>9</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E107" s="1">
         <v>2</v>
@@ -3200,7 +3200,7 @@
         <v>13.2</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E108" s="1">
         <v>8</v>
@@ -3220,7 +3220,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E109" s="1">
         <v>3</v>
@@ -3240,7 +3240,7 @@
         <v>16.5</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E110" s="1">
         <v>5</v>
@@ -3260,7 +3260,7 @@
         <v>9.6</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E111" s="1">
         <v>2</v>
@@ -3280,7 +3280,7 @@
         <v>14.4</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E112" s="1">
         <v>1</v>
@@ -3300,7 +3300,7 @@
         <v>8.5</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E113" s="1">
         <v>6</v>
@@ -3320,7 +3320,7 @@
         <v>12.5</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E114" s="1">
         <v>3</v>
@@ -3340,7 +3340,7 @@
         <v>15.6</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E115" s="1">
         <v>4</v>
@@ -3360,7 +3360,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E116" s="1">
         <v>7</v>
@@ -3380,7 +3380,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E117" s="1">
         <v>2</v>
@@ -3400,7 +3400,7 @@
         <v>11.6</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E118" s="1">
         <v>8</v>
@@ -3420,7 +3420,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E119" s="1">
         <v>7</v>
@@ -3440,7 +3440,7 @@
         <v>15</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E120" s="1">
         <v>6</v>
@@ -3460,7 +3460,7 @@
         <v>12.9</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E121" s="1">
         <v>3</v>
@@ -3480,7 +3480,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E122" s="1">
         <v>1</v>
@@ -3500,7 +3500,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E123" s="1">
         <v>2</v>
@@ -3520,7 +3520,7 @@
         <v>13.4</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E124" s="1">
         <v>8</v>
@@ -3540,7 +3540,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E125" s="1">
         <v>6</v>
@@ -3560,7 +3560,7 @@
         <v>8</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E126" s="1">
         <v>2</v>
@@ -3580,7 +3580,7 @@
         <v>14.1</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E127" s="1">
         <v>8</v>
@@ -3600,7 +3600,7 @@
         <v>9.5</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E128" s="1">
         <v>3</v>
@@ -3620,7 +3620,7 @@
         <v>16.5</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E129" s="1">
         <v>1</v>
@@ -3640,7 +3640,7 @@
         <v>12.4</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E130" s="1">
         <v>7</v>
@@ -3660,7 +3660,7 @@
         <v>18.3</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E131" s="1">
         <v>4</v>
@@ -3680,7 +3680,7 @@
         <v>14</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E132" s="1">
         <v>7</v>
@@ -3700,7 +3700,7 @@
         <v>7.7</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E133" s="1">
         <v>6</v>
@@ -3720,7 +3720,7 @@
         <v>11.4</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E134" s="1">
         <v>8</v>
@@ -3740,7 +3740,7 @@
         <v>15.2</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E135" s="1">
         <v>3</v>
@@ -3760,7 +3760,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E136" s="1">
         <v>4</v>
@@ -3780,7 +3780,7 @@
         <v>18.7</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E137" s="1">
         <v>1</v>
@@ -3800,7 +3800,7 @@
         <v>13.3</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E138" s="1">
         <v>5</v>
@@ -3820,7 +3820,7 @@
         <v>12.6</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E139" s="1">
         <v>4</v>
@@ -3840,7 +3840,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E140" s="1">
         <v>3</v>
@@ -3860,7 +3860,7 @@
         <v>11.2</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E141" s="1">
         <v>7</v>
@@ -3880,7 +3880,7 @@
         <v>15.1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E142" s="1">
         <v>6</v>
@@ -3900,7 +3900,7 @@
         <v>8.9</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E143" s="1">
         <v>2</v>
@@ -3920,7 +3920,7 @@
         <v>14.3</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E144" s="1">
         <v>8</v>
@@ -3940,7 +3940,7 @@
         <v>7.5</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E145" s="1">
         <v>5</v>
@@ -3960,7 +3960,7 @@
         <v>16.8</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E146" s="1">
         <v>6</v>
@@ -3980,7 +3980,7 @@
         <v>12.1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E147" s="1">
         <v>3</v>
@@ -4000,7 +4000,7 @@
         <v>9.1</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E148" s="1">
         <v>4</v>
@@ -4020,7 +4020,7 @@
         <v>13</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E149" s="1">
         <v>7</v>
@@ -4040,7 +4040,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E150" s="1">
         <v>1</v>
@@ -4060,7 +4060,7 @@
         <v>10.6</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E151" s="1">
         <v>8</v>
@@ -4080,7 +4080,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E152" s="1">
         <v>4</v>
@@ -4100,7 +4100,7 @@
         <v>8.4</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E153" s="1">
         <v>2</v>
@@ -4120,7 +4120,7 @@
         <v>15.4</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E154" s="1">
         <v>5</v>
@@ -4140,7 +4140,7 @@
         <v>12</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E155" s="1">
         <v>6</v>
@@ -4160,7 +4160,7 @@
         <v>9.6</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E156" s="1">
         <v>3</v>
@@ -4180,7 +4180,7 @@
         <v>13.8</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E157" s="1">
         <v>7</v>
@@ -4200,7 +4200,7 @@
         <v>19.3</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E158" s="1">
         <v>4</v>
@@ -4220,7 +4220,7 @@
         <v>14.7</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E159" s="1">
         <v>8</v>
@@ -4240,7 +4240,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E160" s="1">
         <v>3</v>
@@ -4260,7 +4260,7 @@
         <v>16</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E161" s="1">
         <v>1</v>
@@ -4280,7 +4280,7 @@
         <v>10.1</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E162" s="1">
         <v>2</v>
@@ -4300,7 +4300,7 @@
         <v>17.7</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E163" s="1">
         <v>7</v>
@@ -4320,7 +4320,7 @@
         <v>12.2</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E164" s="1">
         <v>5</v>
@@ -4340,7 +4340,7 @@
         <v>11.9</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E165" s="1">
         <v>3</v>
@@ -4360,7 +4360,7 @@
         <v>15.5</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E166" s="1">
         <v>6</v>
@@ -4380,7 +4380,7 @@
         <v>8.6</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E167" s="1">
         <v>8</v>
@@ -4400,7 +4400,7 @@
         <v>14.2</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E168" s="1">
         <v>2</v>
@@ -4420,7 +4420,7 @@
         <v>11.3</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E169" s="1">
         <v>4</v>
@@ -4440,7 +4440,7 @@
         <v>10.5</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E170" s="1">
         <v>5</v>
@@ -4460,7 +4460,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E171" s="1">
         <v>2</v>
@@ -4480,7 +4480,7 @@
         <v>13.4</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E172" s="1">
         <v>8</v>
@@ -4500,7 +4500,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E173" s="1">
         <v>6</v>
@@ -4520,7 +4520,7 @@
         <v>18</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E174" s="1">
         <v>7</v>
@@ -4540,7 +4540,7 @@
         <v>14.5</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E175" s="1">
         <v>4</v>
@@ -4560,7 +4560,7 @@
         <v>11.8</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E176" s="1">
         <v>1</v>
@@ -4580,7 +4580,7 @@
         <v>9</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E177" s="1">
         <v>7</v>
@@ -4600,7 +4600,7 @@
         <v>13.2</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E178" s="1">
         <v>4</v>
@@ -4620,7 +4620,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E179" s="1">
         <v>2</v>
@@ -4640,7 +4640,7 @@
         <v>10.9</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E180" s="1">
         <v>8</v>
@@ -4660,7 +4660,7 @@
         <v>15.2</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E181" s="1">
         <v>3</v>
@@ -4680,7 +4680,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E182" s="1">
         <v>6</v>
@@ -4700,7 +4700,7 @@
         <v>16.7</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E183" s="1">
         <v>8</v>
@@ -4720,7 +4720,7 @@
         <v>12.5</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E184" s="1">
         <v>1</v>
@@ -4740,7 +4740,7 @@
         <v>11.7</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E185" s="1">
         <v>5</v>
@@ -4760,7 +4760,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E186" s="1">
         <v>2</v>
@@ -4780,7 +4780,7 @@
         <v>13.5</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E187" s="1">
         <v>4</v>
@@ -4800,7 +4800,7 @@
         <v>18.2</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E188" s="1">
         <v>6</v>
@@ -4820,7 +4820,7 @@
         <v>14.6</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E189" s="1">
         <v>3</v>
@@ -4840,7 +4840,7 @@
         <v>10.4</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E190" s="1">
         <v>8</v>
@@ -4860,7 +4860,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E191" s="1">
         <v>7</v>
@@ -4880,7 +4880,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E192" s="1">
         <v>1</v>
@@ -4900,7 +4900,7 @@
         <v>16.3</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E193" s="1">
         <v>2</v>
@@ -4920,7 +4920,7 @@
         <v>11.1</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E194" s="1">
         <v>8</v>
@@ -4940,7 +4940,7 @@
         <v>15.9</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E195" s="1">
         <v>4</v>
@@ -4960,7 +4960,7 @@
         <v>13.7</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E196" s="1">
         <v>6</v>
@@ -4980,7 +4980,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E197" s="1">
         <v>8</v>
@@ -5000,7 +5000,7 @@
         <v>12.9</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E198" s="1">
         <v>5</v>
@@ -5020,7 +5020,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E199" s="1">
         <v>4</v>
@@ -5040,7 +5040,7 @@
         <v>9.5</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E200" s="1">
         <v>3</v>
@@ -5060,7 +5060,7 @@
         <v>14.3</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E201" s="1">
         <v>7</v>
@@ -5080,7 +5080,7 @@
         <v>11.4</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E202" s="1">
         <v>2</v>
@@ -5100,7 +5100,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E203" s="1">
         <v>1</v>
@@ -5120,7 +5120,7 @@
         <v>15.6</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E204" s="1">
         <v>5</v>
@@ -5140,7 +5140,7 @@
         <v>8.5</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E205" s="1">
         <v>2</v>
@@ -5160,7 +5160,7 @@
         <v>18.3</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E206" s="1">
         <v>7</v>
@@ -5180,7 +5180,7 @@
         <v>13</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E207" s="1">
         <v>3</v>
@@ -5200,7 +5200,7 @@
         <v>12.2</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E208" s="1">
         <v>8</v>
@@ -5220,7 +5220,7 @@
         <v>16.8</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E209" s="1">
         <v>4</v>
@@ -5240,7 +5240,7 @@
         <v>10.7</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E210" s="1">
         <v>1</v>
@@ -5260,7 +5260,7 @@
         <v>14</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E211" s="1">
         <v>6</v>
@@ -5280,7 +5280,7 @@
         <v>11.6</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E212" s="1">
         <v>3</v>
@@ -5300,7 +5300,7 @@
         <v>7.8</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E213" s="1">
         <v>5</v>
@@ -5320,7 +5320,7 @@
         <v>17.2</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E214" s="1">
         <v>1</v>
@@ -5340,7 +5340,7 @@
         <v>13.9</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E215" s="1">
         <v>7</v>
@@ -5360,7 +5360,7 @@
         <v>9.1</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E216" s="1">
         <v>4</v>
@@ -5380,7 +5380,7 @@
         <v>14.5</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E217" s="1">
         <v>2</v>
@@ -5400,7 +5400,7 @@
         <v>11.2</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E218" s="1">
         <v>8</v>
@@ -5420,7 +5420,7 @@
         <v>15.3</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E219" s="1">
         <v>6</v>
@@ -5440,7 +5440,7 @@
         <v>7.5</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E220" s="1">
         <v>7</v>
@@ -5460,7 +5460,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E221" s="1">
         <v>3</v>
@@ -5480,7 +5480,7 @@
         <v>12.3</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E222" s="1">
         <v>4</v>
@@ -5500,7 +5500,7 @@
         <v>10.9</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E223" s="1">
         <v>5</v>
@@ -5520,7 +5520,7 @@
         <v>14.7</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E224" s="1">
         <v>2</v>
@@ -5540,7 +5540,7 @@
         <v>8</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E225" s="1">
         <v>8</v>
@@ -5560,7 +5560,7 @@
         <v>11</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E226" s="1">
         <v>1</v>
@@ -5580,7 +5580,7 @@
         <v>15.8</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E227" s="1">
         <v>6</v>
@@ -5600,7 +5600,7 @@
         <v>9.4</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E228" s="1">
         <v>4</v>
@@ -5620,7 +5620,7 @@
         <v>13.6</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E229" s="1">
         <v>2</v>
@@ -5640,7 +5640,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E230" s="1">
         <v>8</v>
@@ -5660,7 +5660,7 @@
         <v>12.8</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E231" s="1">
         <v>3</v>
@@ -5680,7 +5680,7 @@
         <v>7.1</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E232" s="1">
         <v>7</v>
@@ -5700,7 +5700,7 @@
         <v>17.3</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E233" s="1">
         <v>5</v>
@@ -5720,7 +5720,7 @@
         <v>10.5</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E234" s="1">
         <v>6</v>
@@ -5740,7 +5740,7 @@
         <v>14.9</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E235" s="1">
         <v>1</v>
@@ -5760,7 +5760,7 @@
         <v>11.7</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E236" s="1">
         <v>7</v>
@@ -5780,7 +5780,7 @@
         <v>9.6</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E237" s="1">
         <v>2</v>
@@ -5800,7 +5800,7 @@
         <v>15.4</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E238" s="1">
         <v>4</v>
@@ -5820,7 +5820,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E239" s="1">
         <v>3</v>
@@ -5840,7 +5840,7 @@
         <v>13.1</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E240" s="1">
         <v>8</v>
@@ -5860,7 +5860,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E241" s="1">
         <v>1</v>
@@ -5880,7 +5880,7 @@
         <v>9.9</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E242" s="1">
         <v>7</v>
@@ -5900,7 +5900,7 @@
         <v>14.2</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E243" s="1">
         <v>2</v>
@@ -5920,7 +5920,7 @@
         <v>11.3</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E244" s="1">
         <v>8</v>
@@ -5940,7 +5940,7 @@
         <v>7.9</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E245" s="1">
         <v>5</v>
@@ -5960,7 +5960,7 @@
         <v>16.7</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E246" s="1">
         <v>3</v>
@@ -5980,7 +5980,7 @@
         <v>13.8</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E247" s="1">
         <v>6</v>
@@ -6000,7 +6000,7 @@
         <v>10.6</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E248" s="1">
         <v>1</v>
@@ -6020,7 +6020,7 @@
         <v>15.5</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E249" s="1">
         <v>4</v>
@@ -6040,7 +6040,7 @@
         <v>12.4</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E250" s="1">
         <v>2</v>
@@ -6060,7 +6060,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E251" s="1">
         <v>6</v>
@@ -6080,7 +6080,7 @@
         <v>17.5</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E252" s="1">
         <v>1</v>
@@ -6100,7 +6100,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E253" s="1">
         <v>5</v>
@@ -6120,7 +6120,7 @@
         <v>13</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E254" s="1">
         <v>3</v>
@@ -6140,7 +6140,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E255" s="1">
         <v>7</v>
@@ -6160,7 +6160,7 @@
         <v>11.9</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E256" s="1">
         <v>4</v>
@@ -6180,7 +6180,7 @@
         <v>14.6</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E257" s="1">
         <v>8</v>
@@ -6200,7 +6200,7 @@
         <v>8.5</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E258" s="1">
         <v>3</v>
@@ -6220,7 +6220,7 @@
         <v>16</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E259" s="1">
         <v>2</v>
@@ -6240,7 +6240,7 @@
         <v>12.2</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E260" s="1">
         <v>7</v>
@@ -6260,7 +6260,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E261" s="1">
         <v>6</v>
@@ -6280,7 +6280,7 @@
         <v>14.1</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E262" s="1">
         <v>1</v>
@@ -6300,7 +6300,7 @@
         <v>7.7</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E263" s="1">
         <v>8</v>
@@ -6320,7 +6320,7 @@
         <v>16.5</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E264" s="1">
         <v>4</v>
@@ -6340,7 +6340,7 @@
         <v>13.4</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E265" s="1">
         <v>5</v>
@@ -6360,7 +6360,7 @@
         <v>10.1</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E266" s="1">
         <v>2</v>
@@ -6380,7 +6380,7 @@
         <v>15.2</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E267" s="1">
         <v>3</v>
@@ -6400,7 +6400,7 @@
         <v>8.9</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E268" s="1">
         <v>4</v>
@@ -6420,7 +6420,7 @@
         <v>14.3</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E269" s="1">
         <v>7</v>
@@ -6440,7 +6440,7 @@
         <v>17.8</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E270" s="1">
         <v>8</v>
@@ -6460,7 +6460,7 @@
         <v>11.2</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E271" s="1">
         <v>1</v>
@@ -6480,7 +6480,7 @@
         <v>15.9</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E272" s="1">
         <v>2</v>
@@ -6500,7 +6500,7 @@
         <v>13.6</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E273" s="1">
         <v>6</v>
@@ -6520,7 +6520,7 @@
         <v>8.4</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E274" s="1">
         <v>3</v>
@@ -6540,7 +6540,7 @@
         <v>12</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E275" s="1">
         <v>5</v>
@@ -6560,7 +6560,7 @@
         <v>16.3</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E276" s="1">
         <v>6</v>
@@ -6580,7 +6580,7 @@
         <v>10.6</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E277" s="1">
         <v>2</v>
@@ -6600,7 +6600,7 @@
         <v>14.9</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E278" s="1">
         <v>7</v>
@@ -6620,7 +6620,7 @@
         <v>11.5</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E279" s="1">
         <v>4</v>
@@ -6640,7 +6640,7 @@
         <v>7.9</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E280" s="1">
         <v>1</v>
@@ -6660,7 +6660,7 @@
         <v>17.2</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E281" s="1">
         <v>8</v>
@@ -6680,7 +6680,7 @@
         <v>12.8</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E282" s="1">
         <v>3</v>
@@ -6700,7 +6700,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E283" s="1">
         <v>4</v>
@@ -6720,7 +6720,7 @@
         <v>14</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E284" s="1">
         <v>2</v>
@@ -6740,7 +6740,7 @@
         <v>16.7</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E285" s="1">
         <v>8</v>
@@ -6760,7 +6760,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E286" s="1">
         <v>6</v>
@@ -6780,7 +6780,7 @@
         <v>15.5</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E287" s="1">
         <v>1</v>
@@ -6800,7 +6800,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E288" s="1">
         <v>5</v>
@@ -6820,7 +6820,7 @@
         <v>12.5</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E289" s="1">
         <v>3</v>
@@ -6840,7 +6840,7 @@
         <v>13.3</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E290" s="1">
         <v>7</v>
@@ -6860,7 +6860,7 @@
         <v>11.8</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E291" s="1">
         <v>7</v>
@@ -6880,7 +6880,7 @@
         <v>9.1</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E292" s="1">
         <v>6</v>
@@ -6900,7 +6900,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E293" s="1">
         <v>3</v>
@@ -6920,7 +6920,7 @@
         <v>14.6</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E294" s="1">
         <v>2</v>
@@ -6940,7 +6940,7 @@
         <v>10.9</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E295" s="1">
         <v>4</v>
@@ -6960,7 +6960,7 @@
         <v>15.4</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E296" s="1">
         <v>8</v>
@@ -6980,7 +6980,7 @@
         <v>7.3</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E297" s="1">
         <v>1</v>
@@ -7000,7 +7000,7 @@
         <v>11.6</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E298" s="1">
         <v>5</v>
@@ -7020,7 +7020,7 @@
         <v>13.9</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E299" s="1">
         <v>2</v>
@@ -7040,7 +7040,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E300" s="1">
         <v>8</v>
@@ -7060,7 +7060,7 @@
         <v>15.8</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E301" s="1">
         <v>3</v>
@@ -7080,7 +7080,7 @@
         <v>11</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E302" s="1">
         <v>6</v>
@@ -7100,7 +7100,7 @@
         <v>10.4</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E303" s="1">
         <v>8</v>
@@ -7120,7 +7120,7 @@
         <v>16.5</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E304" s="1">
         <v>4</v>
@@ -7140,7 +7140,7 @@
         <v>8</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E305" s="1">
         <v>7</v>
@@ -7160,7 +7160,7 @@
         <v>12.3</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E306" s="1">
         <v>1</v>
@@ -7180,7 +7180,7 @@
         <v>14.7</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E307" s="1">
         <v>2</v>
@@ -7200,7 +7200,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E308" s="1">
         <v>7</v>
@@ -7220,7 +7220,7 @@
         <v>10.7</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E309" s="1">
         <v>3</v>
@@ -7240,7 +7240,7 @@
         <v>9.5</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E310" s="1">
         <v>4</v>
@@ -7260,7 +7260,7 @@
         <v>13.2</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E311" s="1">
         <v>5</v>
@@ -7280,7 +7280,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E312" s="1">
         <v>8</v>
@@ -7300,7 +7300,7 @@
         <v>11.3</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E313" s="1">
         <v>1</v>
@@ -7320,7 +7320,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E314" s="1">
         <v>6</v>
@@ -7340,7 +7340,7 @@
         <v>14.4</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E315" s="1">
         <v>3</v>
@@ -7360,7 +7360,7 @@
         <v>10</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E316" s="1">
         <v>2</v>
@@ -7380,7 +7380,7 @@
         <v>15.6</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E317" s="1">
         <v>5</v>
@@ -7400,7 +7400,7 @@
         <v>12.1</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E318" s="1">
         <v>1</v>
@@ -7420,7 +7420,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E319" s="1">
         <v>7</v>
@@ -7440,7 +7440,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E320" s="1">
         <v>4</v>
@@ -7460,7 +7460,7 @@
         <v>11.5</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E321" s="1">
         <v>8</v>
@@ -7480,7 +7480,7 @@
         <v>14.1</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E322" s="1">
         <v>2</v>
@@ -7500,7 +7500,7 @@
         <v>7.6</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E323" s="1">
         <v>8</v>
@@ -7520,7 +7520,7 @@
         <v>17.7</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E324" s="1">
         <v>6</v>
@@ -7540,7 +7540,7 @@
         <v>13</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E325" s="1">
         <v>7</v>
@@ -7560,7 +7560,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E326" s="1">
         <v>3</v>
@@ -7580,7 +7580,7 @@
         <v>15.3</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E327" s="1">
         <v>4</v>
@@ -7600,7 +7600,7 @@
         <v>11.9</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E328" s="1">
         <v>5</v>
@@ -7620,7 +7620,7 @@
         <v>8.4</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E329" s="1">
         <v>2</v>
@@ -7640,7 +7640,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E330" s="1">
         <v>1</v>
@@ -7660,7 +7660,7 @@
         <v>12.6</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E331" s="1">
         <v>8</v>
@@ -7680,7 +7680,7 @@
         <v>9</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E332" s="1">
         <v>7</v>
@@ -7700,7 +7700,7 @@
         <v>14.5</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E333" s="1">
         <v>3</v>
@@ -7720,7 +7720,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E334" s="1">
         <v>6</v>
@@ -7740,7 +7740,7 @@
         <v>17.8</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E335" s="1">
         <v>1</v>
@@ -7760,7 +7760,7 @@
         <v>13.3</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E336" s="1">
         <v>4</v>
@@ -7780,7 +7780,7 @@
         <v>10.5</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E337" s="1">
         <v>2</v>
@@ -7800,7 +7800,7 @@
         <v>15.1</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E338" s="1">
         <v>5</v>
@@ -7820,7 +7820,7 @@
         <v>11.2</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E339" s="1">
         <v>6</v>
@@ -7840,7 +7840,7 @@
         <v>7.8</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E340" s="1">
         <v>3</v>
@@ -7860,7 +7860,7 @@
         <v>16</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E341" s="1">
         <v>4</v>
@@ -7880,7 +7880,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E342" s="1">
         <v>7</v>
@@ -7900,7 +7900,7 @@
         <v>13.6</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E343" s="1">
         <v>1</v>
@@ -7920,7 +7920,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E344" s="1">
         <v>8</v>
@@ -7940,7 +7940,7 @@
         <v>12.2</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E345" s="1">
         <v>5</v>
@@ -7960,7 +7960,7 @@
         <v>10.9</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E346" s="1">
         <v>2</v>
@@ -7980,7 +7980,7 @@
         <v>15.7</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E347" s="1">
         <v>7</v>
@@ -8000,7 +8000,7 @@
         <v>8.6</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E348" s="1">
         <v>4</v>
@@ -8020,7 +8020,7 @@
         <v>14.8</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E349" s="1">
         <v>2</v>
@@ -8040,7 +8040,7 @@
         <v>11.4</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E350" s="1">
         <v>8</v>
@@ -8060,7 +8060,7 @@
         <v>9.9</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E351" s="1">
         <v>3</v>
@@ -8080,7 +8080,7 @@
         <v>13.4</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E352" s="1">
         <v>1</v>
@@ -8100,7 +8100,7 @@
         <v>7.2</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E353" s="1">
         <v>6</v>
@@ -8120,7 +8120,7 @@
         <v>16.3</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E354" s="1">
         <v>5</v>
@@ -8140,7 +8140,7 @@
         <v>13.1</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E355" s="1">
         <v>2</v>
@@ -8160,7 +8160,7 @@
         <v>11.6</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E356" s="1">
         <v>7</v>
@@ -8180,7 +8180,7 @@
         <v>9.4</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E357" s="1">
         <v>6</v>
@@ -8200,7 +8200,7 @@
         <v>14.7</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E358" s="1">
         <v>1</v>
@@ -8220,7 +8220,7 @@
         <v>10.1</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E359" s="1">
         <v>8</v>
@@ -8240,7 +8240,7 @@
         <v>15.5</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E360" s="1">
         <v>3</v>
@@ -8260,7 +8260,7 @@
         <v>8</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E361" s="1">
         <v>5</v>
@@ -8280,7 +8280,7 @@
         <v>12.9</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E362" s="1">
         <v>4</v>
@@ -8300,7 +8300,7 @@
         <v>14.2</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E363" s="1">
         <v>8</v>
@@ -8320,7 +8320,7 @@
         <v>11</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E364" s="1">
         <v>1</v>
@@ -8340,7 +8340,7 @@
         <v>16.7</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E365" s="1">
         <v>7</v>
@@ -8360,7 +8360,7 @@
         <v>13.8</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E366" s="1">
         <v>4</v>
@@ -8380,7 +8380,7 @@
         <v>10.3</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E367" s="1">
         <v>2</v>
@@ -8400,7 +8400,7 @@
         <v>15.4</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E368" s="1">
         <v>3</v>
@@ -8420,7 +8420,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E369" s="1">
         <v>5</v>
@@ -8440,7 +8440,7 @@
         <v>11.5</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E370" s="1">
         <v>6</v>
@@ -8460,7 +8460,7 @@
         <v>16.2</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E371" s="1">
         <v>3</v>
@@ -8480,7 +8480,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E372" s="1">
         <v>1</v>
@@ -8500,7 +8500,7 @@
         <v>14.3</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E373" s="1">
         <v>2</v>
@@ -8520,7 +8520,7 @@
         <v>7.4</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E374" s="1">
         <v>7</v>
@@ -8540,7 +8540,7 @@
         <v>16.8</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E375" s="1">
         <v>8</v>
@@ -8560,7 +8560,7 @@
         <v>12</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E376" s="1">
         <v>4</v>
@@ -8580,7 +8580,7 @@
         <v>11.1</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E377" s="1">
         <v>2</v>
@@ -8600,7 +8600,7 @@
         <v>9.5</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E378" s="1">
         <v>8</v>
@@ -8620,7 +8620,7 @@
         <v>13.9</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E379" s="1">
         <v>6</v>
@@ -8640,7 +8640,7 @@
         <v>17.3</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E380" s="1">
         <v>1</v>
@@ -8660,7 +8660,7 @@
         <v>10.6</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E381" s="1">
         <v>7</v>
@@ -8680,7 +8680,7 @@
         <v>15.2</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E382" s="1">
         <v>3</v>
@@ -8700,7 +8700,7 @@
         <v>11.3</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E383" s="1">
         <v>5</v>
@@ -8720,7 +8720,7 @@
         <v>8.1</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E384" s="1">
         <v>4</v>
@@ -8740,7 +8740,7 @@
         <v>14.6</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E385" s="1">
         <v>8</v>
@@ -8760,7 +8760,7 @@
         <v>9.1</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E386" s="1">
         <v>3</v>
@@ -8780,7 +8780,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E387" s="1">
         <v>7</v>
@@ -8800,7 +8800,7 @@
         <v>13.5</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E388" s="1">
         <v>4</v>
@@ -8820,7 +8820,7 @@
         <v>10</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E389" s="1">
         <v>1</v>
@@ -8840,7 +8840,7 @@
         <v>15.7</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E390" s="1">
         <v>6</v>
@@ -8860,7 +8860,7 @@
         <v>11.9</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E391" s="1">
         <v>2</v>
@@ -8880,7 +8880,7 @@
         <v>8.5</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E392" s="1">
         <v>5</v>
@@ -8900,7 +8900,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E393" s="1">
         <v>6</v>
@@ -8920,7 +8920,7 @@
         <v>9.4</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E394" s="1">
         <v>8</v>
@@ -8940,7 +8940,7 @@
         <v>13</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E395" s="1">
         <v>2</v>
@@ -8960,7 +8960,7 @@
         <v>18</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E396" s="1">
         <v>3</v>
@@ -8980,7 +8980,7 @@
         <v>12.3</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E397" s="1">
         <v>1</v>
@@ -9000,7 +9000,7 @@
         <v>7.7</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E398" s="1">
         <v>7</v>
@@ -9020,7 +9020,7 @@
         <v>14.9</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E399" s="1">
         <v>5</v>
@@ -9040,7 +9040,7 @@
         <v>11.7</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E400" s="1">
         <v>4</v>
@@ -9060,7 +9060,7 @@
         <v>10.1</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E401" s="1">
         <v>7</v>
@@ -9080,7 +9080,7 @@
         <v>15.6</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E402" s="1">
         <v>1</v>
@@ -9100,7 +9100,7 @@
         <v>8.9</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E403" s="1">
         <v>8</v>
@@ -9120,7 +9120,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E404" s="1">
         <v>3</v>
@@ -9140,7 +9140,7 @@
         <v>13.8</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E405" s="1">
         <v>6</v>
@@ -9160,7 +9160,7 @@
         <v>10.4</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E406" s="1">
         <v>5</v>
@@ -9180,7 +9180,7 @@
         <v>15.3</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E407" s="1">
         <v>2</v>
@@ -9200,7 +9200,7 @@
         <v>11.2</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E408" s="1">
         <v>4</v>
@@ -9220,7 +9220,7 @@
         <v>8.6</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E409" s="1">
         <v>7</v>
@@ -9240,7 +9240,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E410" s="1">
         <v>2</v>
@@ -9260,7 +9260,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E411" s="1">
         <v>8</v>
@@ -9280,7 +9280,7 @@
         <v>14.5</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E412" s="1">
         <v>6</v>
@@ -9300,7 +9300,7 @@
         <v>12.6</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E413" s="1">
         <v>3</v>
@@ -9320,7 +9320,7 @@
         <v>10.8</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E414" s="1">
         <v>1</v>
@@ -9340,7 +9340,7 @@
         <v>15.9</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E415" s="1">
         <v>4</v>
@@ -9360,7 +9360,7 @@
         <v>7.9</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E416" s="1">
         <v>5</v>
@@ -9380,7 +9380,7 @@
         <v>13.2</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E417" s="1">
         <v>3</v>
@@ -9400,7 +9400,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E418" s="1">
         <v>6</v>
@@ -9420,7 +9420,7 @@
         <v>11.5</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E419" s="1">
         <v>8</v>
@@ -9440,7 +9440,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E420" s="1">
         <v>1</v>
@@ -9460,7 +9460,7 @@
         <v>14.7</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E421" s="1">
         <v>2</v>
@@ -9480,7 +9480,7 @@
         <v>10</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E422" s="1">
         <v>7</v>
@@ -9500,7 +9500,7 @@
         <v>15.4</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E423" s="1">
         <v>4</v>
@@ -9520,7 +9520,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E424" s="1">
         <v>2</v>
@@ -9540,7 +9540,7 @@
         <v>12.9</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E425" s="1">
         <v>8</v>
@@ -9560,7 +9560,7 @@
         <v>17.5</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E426" s="1">
         <v>3</v>
@@ -9580,7 +9580,7 @@
         <v>11.1</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E427" s="1">
         <v>5</v>
@@ -9600,7 +9600,7 @@
         <v>16.2</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E428" s="1">
         <v>4</v>
@@ -9620,7 +9620,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E429" s="1">
         <v>1</v>
@@ -9640,7 +9640,7 @@
         <v>13.6</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E430" s="1">
         <v>7</v>
@@ -9660,7 +9660,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E431" s="1">
         <v>6</v>
@@ -9680,7 +9680,7 @@
         <v>14.4</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E432" s="1">
         <v>2</v>
@@ -9700,7 +9700,7 @@
         <v>7.3</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E433" s="1">
         <v>8</v>
@@ -9720,7 +9720,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E434" s="1">
         <v>3</v>
@@ -9740,7 +9740,7 @@
         <v>12.2</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E435" s="1">
         <v>7</v>
@@ -9760,7 +9760,7 @@
         <v>11.5</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E436" s="1">
         <v>1</v>
@@ -9780,7 +9780,7 @@
         <v>9</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E437" s="1">
         <v>6</v>
@@ -9800,7 +9800,7 @@
         <v>13.4</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E438" s="1">
         <v>4</v>
@@ -9820,7 +9820,7 @@
         <v>17.7</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E439" s="1">
         <v>5</v>

</xml_diff>